<commit_message>
EXCEL Y WORD LLENOS
</commit_message>
<xml_diff>
--- a/Docs/TablasDatos-Lab4.xlsx
+++ b/Docs/TablasDatos-Lab4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/2021-20/Laboratorios/Lab 04 - Ordenamientos Iter + Rec/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Cosas Pipe\Andes\Semestre 3\EDA\LabSorts-S04-G01\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F3EF8E-9153-42A5-8ACF-6285D7DFF156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5B8DD7-2CBE-45E1-9A2F-A87B23AA703B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="6" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4-5" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,7 +556,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -623,7 +623,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -711,7 +711,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -756,28 +756,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>15.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>187.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>781.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>3250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75</c:v>
+                  <c:v>7812.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
+                  <c:v>20765.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105</c:v>
+                  <c:v>54171.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120</c:v>
+                  <c:v>84531.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,7 +874,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -919,28 +919,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>78.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>140.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>265.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>406.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>531.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1037,7 +1037,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1082,28 +1082,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>46.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>203.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>421.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>140</c:v>
+                  <c:v>968.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160</c:v>
+                  <c:v>1453.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1199,28 +1199,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>109.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>210</c:v>
+                  <c:v>203.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>328.125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>270</c:v>
+                  <c:v>406.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1320,7 +1320,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1358,7 +1358,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1442,7 +1442,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1480,7 +1480,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1522,7 +1522,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1559,7 +1559,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1568,7 +1568,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1635,7 +1635,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1732,7 +1732,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1777,16 +1777,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>7125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>60515.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>484126</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>90</c:v>
@@ -1887,7 +1887,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1932,28 +1932,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>546.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>12500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>12510</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>118</c:v>
+                  <c:v>12520</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>128</c:v>
+                  <c:v>12530</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>138</c:v>
+                  <c:v>12540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2050,7 +2050,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2095,16 +2095,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>531.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>2484.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>12420</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>150</c:v>
@@ -2213,7 +2213,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2258,16 +2258,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>78.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>281.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>983.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>150</c:v>
@@ -2379,7 +2379,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2417,7 +2417,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -2501,7 +2501,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2539,7 +2539,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -2581,7 +2581,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2618,7 +2618,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2627,7 +2627,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2694,7 +2694,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2781,7 +2781,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2826,28 +2826,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>15.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>187.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>781.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>3250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>75</c:v>
+                  <c:v>7812.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
+                  <c:v>20765.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105</c:v>
+                  <c:v>54171.875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120</c:v>
+                  <c:v>84531.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2936,7 +2936,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2981,16 +2981,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>7125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>60515.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>484126</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>90</c:v>
@@ -3102,7 +3102,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3140,7 +3140,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3219,7 +3219,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3257,7 +3257,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3299,7 +3299,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3336,7 +3336,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3345,7 +3345,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3415,7 +3415,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3502,7 +3502,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3547,28 +3547,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>78.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>140.625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>265.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>406.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>531.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3657,7 +3657,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3702,28 +3702,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>546.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>12500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
+                  <c:v>12510</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>118</c:v>
+                  <c:v>12520</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>128</c:v>
+                  <c:v>12530</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>138</c:v>
+                  <c:v>12540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3823,7 +3823,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3861,7 +3861,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3940,7 +3940,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3978,7 +3978,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4020,7 +4020,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4057,7 +4057,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -4066,7 +4066,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4136,7 +4136,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4223,7 +4223,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4268,28 +4268,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>46.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>93.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>203.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120</c:v>
+                  <c:v>421.875</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>140</c:v>
+                  <c:v>968.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160</c:v>
+                  <c:v>1453.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4378,7 +4378,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4423,16 +4423,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>531.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>2484.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>12420</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>150</c:v>
@@ -4544,7 +4544,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4582,7 +4582,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4661,7 +4661,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4699,7 +4699,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4741,7 +4741,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4778,7 +4778,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -4787,7 +4787,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4857,7 +4857,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4945,7 +4945,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4990,28 +4990,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>15.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>150</c:v>
+                  <c:v>62.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>109.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>210</c:v>
+                  <c:v>203.125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>328.125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>270</c:v>
+                  <c:v>406.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5101,7 +5101,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5146,16 +5146,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>78.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>281.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>983.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>150</c:v>
@@ -5267,7 +5267,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5305,7 +5305,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -5384,7 +5384,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5422,7 +5422,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -5464,7 +5464,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5501,7 +5501,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -8852,7 +8852,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8874,7 +8874,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8885,7 +8885,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C0D6BB1E-4928-4857-A0CD-C818D0A5A6F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8896,7 +8896,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B3AE6AD4-6EB7-44ED-A987-5D4A68E7E10B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8907,7 +8907,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661768" cy="6283739"/>
+    <xdr:ext cx="9301370" cy="6071152"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8940,7 +8940,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -8973,7 +8973,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661400" cy="6286500"/>
+    <xdr:ext cx="9305925" cy="6076950"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -9006,7 +9006,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -9039,7 +9039,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -9072,7 +9072,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9290137" cy="6067295"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -9136,7 +9136,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9434,21 +9434,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.17578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.46875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.41015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.64453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.87890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" ht="27.35" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="8" customFormat="1" ht="28.5">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -9468,7 +9468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6">
       <c r="A2" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -9477,19 +9477,19 @@
         <v>50</v>
       </c>
       <c r="C2" s="3">
-        <v>15.7</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F2" s="4">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6">
       <c r="A3" s="5">
         <v>0.05</v>
       </c>
@@ -9498,20 +9498,19 @@
         <v>500</v>
       </c>
       <c r="C3" s="3">
-        <v>30</v>
+        <v>187.5</v>
       </c>
       <c r="D3" s="3">
-        <f>D2+15</f>
-        <v>19</v>
+        <v>15.625</v>
       </c>
       <c r="E3" s="4">
-        <v>40</v>
+        <v>31.25</v>
       </c>
       <c r="F3" s="4">
-        <v>90</v>
+        <v>15.625</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6">
       <c r="A4" s="5">
         <v>0.1</v>
       </c>
@@ -9520,20 +9519,19 @@
         <v>1000</v>
       </c>
       <c r="C4" s="3">
-        <v>45</v>
+        <v>781.25</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D9" si="0">D3+10</f>
-        <v>29</v>
+        <v>31.25</v>
       </c>
       <c r="E4" s="4">
-        <v>60</v>
+        <v>46.875</v>
       </c>
       <c r="F4" s="4">
-        <v>120</v>
+        <v>31.25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6">
       <c r="A5" s="5">
         <v>0.2</v>
       </c>
@@ -9542,20 +9540,19 @@
         <v>2000</v>
       </c>
       <c r="C5" s="3">
-        <v>60</v>
+        <v>3250</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <v>78.125</v>
       </c>
       <c r="E5" s="4">
-        <v>80</v>
+        <v>93.75</v>
       </c>
       <c r="F5" s="4">
-        <v>150</v>
+        <v>62.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6">
       <c r="A6" s="5">
         <v>0.3</v>
       </c>
@@ -9564,20 +9561,19 @@
         <v>3000</v>
       </c>
       <c r="C6" s="3">
-        <v>75</v>
+        <v>7812.5</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <v>140.625</v>
       </c>
       <c r="E6" s="4">
-        <v>100</v>
+        <v>203.25</v>
       </c>
       <c r="F6" s="4">
-        <v>180</v>
+        <v>109.375</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6">
       <c r="A7" s="5">
         <v>0.5</v>
       </c>
@@ -9586,20 +9582,19 @@
         <v>5000</v>
       </c>
       <c r="C7" s="3">
-        <v>90</v>
+        <v>20765.625</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <v>265.625</v>
       </c>
       <c r="E7" s="4">
-        <v>120</v>
+        <v>421.875</v>
       </c>
       <c r="F7" s="4">
-        <v>210</v>
+        <v>203.125</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6">
       <c r="A8" s="5">
         <v>0.8</v>
       </c>
@@ -9608,20 +9603,19 @@
         <v>8000</v>
       </c>
       <c r="C8" s="3">
-        <v>105</v>
+        <v>54171.875</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>69</v>
+        <v>406.25</v>
       </c>
       <c r="E8" s="4">
-        <v>140</v>
+        <v>968.75</v>
       </c>
       <c r="F8" s="4">
-        <v>240</v>
+        <v>328.125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -9630,20 +9624,19 @@
         <v>10000</v>
       </c>
       <c r="C9" s="3">
-        <v>120</v>
+        <v>84531.25</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <v>531.25</v>
       </c>
       <c r="E9" s="4">
-        <v>160</v>
+        <v>1453.125</v>
       </c>
       <c r="F9" s="4">
-        <v>270</v>
+        <v>406.25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="8" customFormat="1" ht="27.35" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" s="8" customFormat="1" ht="28.5">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
@@ -9663,7 +9656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6">
       <c r="A13" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -9672,19 +9665,19 @@
         <v>50</v>
       </c>
       <c r="C13" s="3">
-        <v>50</v>
+        <v>15.625</v>
       </c>
       <c r="D13" s="3">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E13" s="4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F13" s="4">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6">
       <c r="A14" s="5">
         <v>0.05</v>
       </c>
@@ -9693,20 +9686,19 @@
         <v>500</v>
       </c>
       <c r="C14" s="3">
-        <v>60</v>
+        <v>7125</v>
       </c>
       <c r="D14" s="3">
-        <f>D13+43</f>
-        <v>78</v>
+        <v>546.875</v>
       </c>
       <c r="E14" s="4">
-        <v>60</v>
+        <v>531.25</v>
       </c>
       <c r="F14" s="4">
-        <v>90</v>
+        <v>78.125</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6">
       <c r="A15" s="5">
         <v>0.1</v>
       </c>
@@ -9715,20 +9707,19 @@
         <v>1000</v>
       </c>
       <c r="C15" s="3">
-        <v>70</v>
+        <v>60515.625</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" ref="D15:D20" si="1">D14+10</f>
-        <v>88</v>
+        <v>2500</v>
       </c>
       <c r="E15" s="4">
-        <v>90</v>
+        <v>2484.375</v>
       </c>
       <c r="F15" s="4">
-        <v>110</v>
+        <v>281.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6">
       <c r="A16" s="5">
         <v>0.2</v>
       </c>
@@ -9737,20 +9728,19 @@
         <v>2000</v>
       </c>
       <c r="C16" s="3">
-        <v>80</v>
+        <v>484126</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="1"/>
-        <v>98</v>
+        <v>12500</v>
       </c>
       <c r="E16" s="4">
-        <v>120</v>
+        <v>12420</v>
       </c>
       <c r="F16" s="4">
-        <v>130</v>
+        <v>983.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6">
       <c r="A17" s="5">
         <v>0.3</v>
       </c>
@@ -9762,8 +9752,8 @@
         <v>90</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="1"/>
-        <v>108</v>
+        <f t="shared" ref="D15:D20" si="0">D16+10</f>
+        <v>12510</v>
       </c>
       <c r="E17" s="4">
         <v>150</v>
@@ -9772,7 +9762,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6">
       <c r="A18" s="5">
         <v>0.5</v>
       </c>
@@ -9784,8 +9774,8 @@
         <v>100</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="1"/>
-        <v>118</v>
+        <f t="shared" si="0"/>
+        <v>12520</v>
       </c>
       <c r="E18" s="4">
         <v>180</v>
@@ -9794,7 +9784,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:6">
       <c r="A19" s="5">
         <v>0.8</v>
       </c>
@@ -9806,8 +9796,8 @@
         <v>110</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="1"/>
-        <v>128</v>
+        <f t="shared" si="0"/>
+        <v>12530</v>
       </c>
       <c r="E19" s="4">
         <v>210</v>
@@ -9816,7 +9806,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6">
       <c r="A20" s="5">
         <v>1</v>
       </c>
@@ -9828,8 +9818,8 @@
         <v>120</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="1"/>
-        <v>138</v>
+        <f t="shared" si="0"/>
+        <v>12540</v>
       </c>
       <c r="E20" s="4">
         <v>240</v>
@@ -9848,112 +9838,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
-      <UserInfo>
-        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
-        <AccountId>50</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Arturo Henao Chaparro</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan Carlos Marin Morales</DisplayName>
-        <AccountId>53</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sofia Duque Gomez</DisplayName>
-        <AccountId>60</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Andres Felipe Romero Brand</DisplayName>
-        <AccountId>91</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
-        <AccountId>92</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
-        <AccountId>94</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Juan David Diaz Ipuz</DisplayName>
-        <AccountId>90</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Isaac David Bermudez Lara</DisplayName>
-        <AccountId>95</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
-        <AccountId>55</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
-        <AccountId>97</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kevin Cohen Solano</DisplayName>
-        <AccountId>93</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
-        <AccountId>96</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10174,15 +10064,142 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
+      <UserInfo>
+        <DisplayName>Carlos Andres Lozano Garzon</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dario Ernesto Correal Torres</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mario  Fernando De la rosa Rosero</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Christian Camilo Aparicio Baquen</DisplayName>
+        <AccountId>50</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Arturo Henao Chaparro</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Luis Esteban Florez Salamanca</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ivan David Salazar Cardenas</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan Carlos Marin Morales</DisplayName>
+        <AccountId>53</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sofia Duque Gomez</DisplayName>
+        <AccountId>60</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Andres Felipe Romero Brand</DisplayName>
+        <AccountId>91</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lindsay Vanessa Pinto Morato</DisplayName>
+        <AccountId>92</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Miguel Angel Acosta Walteros</DisplayName>
+        <AccountId>94</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Juan David Diaz Ipuz</DisplayName>
+        <AccountId>90</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lily Aitana valentina Duque Chavez</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Isaac David Bermudez Lara</DisplayName>
+        <AccountId>95</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Daniel Alejandro Angel Fuertes</DisplayName>
+        <AccountId>55</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeniffer Liliam Mendoza Espinosa</DisplayName>
+        <AccountId>97</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kevin Cohen Solano</DisplayName>
+        <AccountId>93</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cesar Luis Moreno Gonzalez</DisplayName>
+        <AccountId>96</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jose Cristobal Arroyo Castellanos</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3198979-0B27-4D27-8331-28B531282E06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -10197,16 +10214,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3198979-0B27-4D27-8331-28B531282E06}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>